<commit_message>
Updated the json_helper to replace datatype short codes with detail datatypes in the generated JSON
</commit_message>
<xml_diff>
--- a/doc/json_helper.xlsx
+++ b/doc/json_helper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace-python\ebcdic\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DC2040-80C2-4D65-8D35-D564B35C14EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEF63E8-FAAF-4577-BA77-3D517A593601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6BC73A61-38C3-47EC-9F53-CCC2817EEE56}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="154">
   <si>
     <t>name</t>
   </si>
@@ -418,24 +418,6 @@
     <t>G-GRAV,PD,3,3</t>
   </si>
   <si>
-    <t>EXC-14B2-TYPE</t>
-  </si>
-  <si>
-    <t>G-1-DATE</t>
-  </si>
-  <si>
-    <t>OPEN-FLO</t>
-  </si>
-  <si>
-    <t>SLOPE</t>
-  </si>
-  <si>
-    <t>RATIO</t>
-  </si>
-  <si>
-    <t>G-GRAV</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -552,6 +534,231 @@
   </si>
   <si>
     <t>Below is sample from page 13 of the above pdf file, in the left side and the corresponding text after adding the datatype short codes and field size and scale size. Colored in Red</t>
+  </si>
+  <si>
+    <t>WELL-REC-TYPE-REC</t>
+  </si>
+  <si>
+    <t>WELL-REC-DIST</t>
+  </si>
+  <si>
+    <t>WELL-REC-FIELD</t>
+  </si>
+  <si>
+    <t>WELL-REC-OPR</t>
+  </si>
+  <si>
+    <t>WELL-REC-LEASE</t>
+  </si>
+  <si>
+    <t>WELL-REC-FILLER</t>
+  </si>
+  <si>
+    <t>WELL-REC-OFFSHORE</t>
+  </si>
+  <si>
+    <t>WELL-NO</t>
+  </si>
+  <si>
+    <t>W-TYPE-WELL</t>
+  </si>
+  <si>
+    <t>W-UNIT-NO</t>
+  </si>
+  <si>
+    <t>W-UNIT-VALUE</t>
+  </si>
+  <si>
+    <t>W-KEY</t>
+  </si>
+  <si>
+    <t>W-COUNTY</t>
+  </si>
+  <si>
+    <t>PUMP</t>
+  </si>
+  <si>
+    <t>W-SP</t>
+  </si>
+  <si>
+    <t>W-N-CODE</t>
+  </si>
+  <si>
+    <t>W-N-AMT</t>
+  </si>
+  <si>
+    <t>W-DEPTH</t>
+  </si>
+  <si>
+    <t>SAND</t>
+  </si>
+  <si>
+    <t>FROZEN</t>
+  </si>
+  <si>
+    <t>PERF</t>
+  </si>
+  <si>
+    <t>W-DATE</t>
+  </si>
+  <si>
+    <t>EX-14B-CD</t>
+  </si>
+  <si>
+    <t>W-SUB-WELL</t>
+  </si>
+  <si>
+    <t>W-NO-PROD-CD</t>
+  </si>
+  <si>
+    <t>W-DELQ-FORM</t>
+  </si>
+  <si>
+    <t>W-TST-EFF</t>
+  </si>
+  <si>
+    <t>W-EXC-TST</t>
+  </si>
+  <si>
+    <t>W-WATER</t>
+  </si>
+  <si>
+    <t>EX-14B-DATE</t>
+  </si>
+  <si>
+    <t>W-RMKS</t>
+  </si>
+  <si>
+    <t>BONUS-CD3</t>
+  </si>
+  <si>
+    <t>BONUS</t>
+  </si>
+  <si>
+    <t>FROZTSF</t>
+  </si>
+  <si>
+    <t>W-WLSD</t>
+  </si>
+  <si>
+    <t>W-TST-DT</t>
+  </si>
+  <si>
+    <t>W-DTE-LST-UTL</t>
+  </si>
+  <si>
+    <t>W-NEW-WB-EXC</t>
+  </si>
+  <si>
+    <t>W-NEW-WB-CONNECT-DATE</t>
+  </si>
+  <si>
+    <t>W-14B2-TYPE-COVERAGE</t>
+  </si>
+  <si>
+    <t>W-14B2-APP-NO</t>
+  </si>
+  <si>
+    <t>FILLER1</t>
+  </si>
+  <si>
+    <t>FILLER2</t>
+  </si>
+  <si>
+    <t>14----W-MONTH-DATE</t>
+  </si>
+  <si>
+    <t>WM-CHG</t>
+  </si>
+  <si>
+    <t>WM-NO</t>
+  </si>
+  <si>
+    <t>WM-ALLOW</t>
+  </si>
+  <si>
+    <t>WM-ACODE</t>
+  </si>
+  <si>
+    <t>WM-TCODE</t>
+  </si>
+  <si>
+    <t>WM-LIMIT</t>
+  </si>
+  <si>
+    <t>WM-ALLOW2</t>
+  </si>
+  <si>
+    <t>WM-ACODE2</t>
+  </si>
+  <si>
+    <t>WM-TCODE2</t>
+  </si>
+  <si>
+    <t>WM-LIMIT2</t>
+  </si>
+  <si>
+    <t>WM-DATE2</t>
+  </si>
+  <si>
+    <t>WM-ALLOW3</t>
+  </si>
+  <si>
+    <t>WM-ACODE3</t>
+  </si>
+  <si>
+    <t>WM-TCODE3</t>
+  </si>
+  <si>
+    <t>WM-LIMIT3</t>
+  </si>
+  <si>
+    <t>WM-DATE3</t>
+  </si>
+  <si>
+    <t>WM-FORM-LCK</t>
+  </si>
+  <si>
+    <t>WM-PGT</t>
+  </si>
+  <si>
+    <t>WM-TSWA</t>
+  </si>
+  <si>
+    <t>WM-EGT</t>
+  </si>
+  <si>
+    <t>WM-ESWA</t>
+  </si>
+  <si>
+    <t>WM-ACRE</t>
+  </si>
+  <si>
+    <t>WM-POTE</t>
+  </si>
+  <si>
+    <t>WM-ACFT</t>
+  </si>
+  <si>
+    <t>WM-GOR</t>
+  </si>
+  <si>
+    <t>WM-OTRAN-CD</t>
+  </si>
+  <si>
+    <t>WM-POT</t>
+  </si>
+  <si>
+    <t>WM-EOT</t>
+  </si>
+  <si>
+    <t>WM-JOHN</t>
+  </si>
+  <si>
+    <t>WM-OOIP</t>
+  </si>
+  <si>
+    <t>----14-FILLER3</t>
   </si>
 </sst>
 </file>
@@ -602,11 +809,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,17 +1137,17 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1064,7 +1272,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -1124,12 +1332,12 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1140,11 +1348,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238E3804-54DC-4735-96AF-8C86A4CBACA9}">
-  <dimension ref="A1:G157"/>
+  <dimension ref="A1:G160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1171,45 +1377,45 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" t="str">
         <f>VLOOKUP(B2,datatypes!B:D,3,0)</f>
-        <v>string</v>
+        <v>uinteger</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G20" si="0">IF(LEN(A2)&gt;0,"				{ ""name"": """&amp;A2&amp;""", ""type"": """&amp;B2&amp;""", ""size"": "&amp;C2&amp;IF(LEN(D2)&gt;0,", ""scale"": "&amp;D2,"")&amp;" },","")</f>
-        <v xml:space="preserve">				{ "name": "EXC-14B2-TYPE", "type": "S", "size": 1 },</v>
+        <f>IF(LEN(A2)&gt;0,"				{ ""name"": """&amp;A2&amp;""", ""type"": """&amp;E2&amp;""", ""size"": "&amp;C2&amp;IF(LEN(D2)&gt;0,", ""scale"": "&amp;D2,"")&amp;" },","")</f>
+        <v xml:space="preserve">				{ "name": "WELL-REC-TYPE-REC", "type": "uinteger", "size": 1 },</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" t="str">
         <f>VLOOKUP(B3,datatypes!B:D,3,0)</f>
         <v>string</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">				{ "name": "FILLER", "type": "S", "size": 1 },</v>
+        <f t="shared" ref="G3:G66" si="0">IF(LEN(A3)&gt;0,"				{ ""name"": """&amp;A3&amp;""", ""type"": """&amp;E3&amp;""", ""size"": "&amp;C3&amp;IF(LEN(D3)&gt;0,", ""scale"": "&amp;D3,"")&amp;" },","")</f>
+        <v xml:space="preserve">				{ "name": "WELL-REC-DIST", "type": "string", "size": 3 },</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -1223,788 +1429,1442 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">				{ "name": "G-1-DATE", "type": "UI", "size": 8 },</v>
+        <v xml:space="preserve">				{ "name": "WELL-REC-FIELD", "type": "uinteger", "size": 8 },</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E5" t="str">
         <f>VLOOKUP(B5,datatypes!B:D,3,0)</f>
-        <v>packedDecimal</v>
+        <v>uinteger</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">				{ "name": "OPEN-FLO", "type": "PD", "size": 7, "scale": 0 },</v>
+        <v xml:space="preserve">				{ "name": "WELL-REC-OPR", "type": "uinteger", "size": 6 },</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
       <c r="E6" t="str">
         <f>VLOOKUP(B6,datatypes!B:D,3,0)</f>
-        <v>packedDecimal</v>
+        <v>uinteger</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">				{ "name": "SLOPE", "type": "PD", "size": 5, "scale": 4 },</v>
+        <v xml:space="preserve">				{ "name": "WELL-REC-LEASE", "type": "uinteger", "size": 5 },</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" t="str">
         <f>VLOOKUP(B7,datatypes!B:D,3,0)</f>
-        <v>packedDecimal</v>
+        <v>uinteger</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">				{ "name": "RATIO", "type": "PD", "size": 5, "scale": 0 },</v>
+        <v xml:space="preserve">				{ "name": "WELL-REC-FILLER", "type": "uinteger", "size": 2 },</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" t="str">
         <f>VLOOKUP(B8,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WELL-REC-OFFSHORE", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="E9" t="str">
+        <f>VLOOKUP(B9,datatypes!B:D,3,0)</f>
+        <v>string</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WELL-NO", "type": "string", "size": 6 },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="str">
+        <f>VLOOKUP(B10,datatypes!B:D,3,0)</f>
+        <v>string</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-TYPE-WELL", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="str">
+        <f>VLOOKUP(B11,datatypes!B:D,3,0)</f>
+        <v>string</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-UNIT-NO", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="str">
+        <f>VLOOKUP(B12,datatypes!B:D,3,0)</f>
+        <v>decimal</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-UNIT-VALUE", "type": "decimal", "size": 4, "scale": 3 },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="str">
+        <f>VLOOKUP(B13,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-KEY", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="str">
+        <f>VLOOKUP(B14,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-COUNTY", "type": "uinteger", "size": 3 },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="str">
+        <f>VLOOKUP(B15,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "PUMP", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="E16" t="str">
+        <f>VLOOKUP(B16,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-SP", "type": "uinteger", "size": 5 },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="str">
+        <f>VLOOKUP(B17,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-N-CODE", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="E18" t="str">
+        <f>VLOOKUP(B18,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-N-AMT", "type": "uinteger", "size": 5 },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="E19" t="str">
+        <f>VLOOKUP(B19,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-DEPTH", "type": "uinteger", "size": 5 },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="str">
+        <f>VLOOKUP(B20,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "SAND", "type": "uinteger", "size": 3 },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="E21" t="str">
+        <f>VLOOKUP(B21,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "FROZEN", "type": "uinteger", "size": 5 },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="E22" t="str">
+        <f>VLOOKUP(B22,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "PERF", "type": "uinteger", "size": 5 },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="E23" t="str">
+        <f>VLOOKUP(B23,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-DATE", "type": "uinteger", "size": 8 },</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="str">
+        <f>VLOOKUP(B24,datatypes!B:D,3,0)</f>
+        <v>string</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "EX-14B-CD", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="str">
+        <f>VLOOKUP(B25,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-SUB-WELL", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="str">
+        <f>VLOOKUP(B26,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-NO-PROD-CD", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="str">
+        <f>VLOOKUP(B27,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-DELQ-FORM", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="str">
+        <f>VLOOKUP(B28,datatypes!B:D,3,0)</f>
+        <v>string</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-TST-EFF", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="str">
+        <f>VLOOKUP(B29,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-EXC-TST", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="E30" t="str">
+        <f>VLOOKUP(B30,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-WATER", "type": "uinteger", "size": 4 },</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="E31" t="str">
+        <f>VLOOKUP(B31,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "EX-14B-DATE", "type": "uinteger", "size": 6 },</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="E32" t="str">
+        <f>VLOOKUP(B32,datatypes!B:D,3,0)</f>
+        <v>string</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-RMKS", "type": "string", "size": 15 },</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="str">
+        <f>VLOOKUP(B33,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "BONUS-CD3", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="E34" t="str">
+        <f>VLOOKUP(B34,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "BONUS", "type": "uinteger", "size": 4 },</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="E35" t="str">
+        <f>VLOOKUP(B35,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "FROZTSF", "type": "uinteger", "size": 3 },</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="str">
+        <f>VLOOKUP(B36,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-WLSD", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="E37" t="str">
+        <f>VLOOKUP(B37,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-TST-DT", "type": "uinteger", "size": 8 },</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="E38" t="str">
+        <f>VLOOKUP(B38,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-DTE-LST-UTL", "type": "uinteger", "size": 6 },</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="str">
+        <f>VLOOKUP(B39,datatypes!B:D,3,0)</f>
+        <v>string</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-NEW-WB-EXC", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="E40" t="str">
+        <f>VLOOKUP(B40,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-NEW-WB-CONNECT-DATE", "type": "uinteger", "size": 8 },</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="str">
+        <f>VLOOKUP(B41,datatypes!B:D,3,0)</f>
+        <v>string</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-14B2-TYPE-COVERAGE", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="E42" t="str">
+        <f>VLOOKUP(B42,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "W-14B2-APP-NO", "type": "uinteger", "size": 6 },</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="E43" t="str">
+        <f>VLOOKUP(B43,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "FILLER", "type": "uinteger", "size": 4 },</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44">
+        <v>18</v>
+      </c>
+      <c r="E44" t="str">
+        <f>VLOOKUP(B44,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "FILLER1", "type": "uinteger", "size": 18 },</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="E45" t="str">
+        <f>VLOOKUP(B45,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "FILLER2", "type": "uinteger", "size": 7 },</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="E46" t="str">
+        <f>VLOOKUP(B46,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "14----W-MONTH-DATE", "type": "uinteger", "size": 6 },</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="E47" t="str">
+        <f>VLOOKUP(B47,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-CHG", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="E48" t="str">
+        <f>VLOOKUP(B48,datatypes!B:D,3,0)</f>
+        <v>uinteger</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-NO", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49" t="str">
+        <f>VLOOKUP(B49,datatypes!B:D,3,0)</f>
         <v>packedDecimal</v>
       </c>
-      <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">				{ "name": "G-GRAV", "type": "PD", "size": 3, "scale": 3 },</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E9" t="e">
-        <f>VLOOKUP(B9,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E10" t="e">
-        <f>VLOOKUP(B10,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E11" t="e">
-        <f>VLOOKUP(B11,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E12" t="e">
-        <f>VLOOKUP(B12,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E13" t="e">
-        <f>VLOOKUP(B13,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E14" t="e">
-        <f>VLOOKUP(B14,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E15" t="e">
-        <f>VLOOKUP(B15,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E16" t="e">
-        <f>VLOOKUP(B16,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E17" t="e">
-        <f>VLOOKUP(B17,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E18" t="e">
-        <f>VLOOKUP(B18,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E19" t="e">
-        <f>VLOOKUP(B19,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E20" t="e">
-        <f>VLOOKUP(B20,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E21" t="e">
-        <f>VLOOKUP(B21,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G21" t="str">
-        <f>IF(LEN(A21)&gt;0,"				{ ""name"": """&amp;A21&amp;""", ""type"": """&amp;B21&amp;""", ""size"": "&amp;C21&amp;IF(LEN(D21)&gt;0,", ""scale"": "&amp;D21,"")&amp;" },","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E22" t="e">
-        <f>VLOOKUP(B22,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G22" t="str">
-        <f t="shared" ref="G22:G85" si="1">IF(LEN(A22)&gt;0,"				{ ""name"": """&amp;A22&amp;""", ""type"": """&amp;B22&amp;""", ""size"": "&amp;C22&amp;IF(LEN(D22)&gt;0,", ""scale"": "&amp;D22,"")&amp;" },","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E23" t="e">
-        <f>VLOOKUP(B23,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E24" t="e">
-        <f>VLOOKUP(B24,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E25" t="e">
-        <f>VLOOKUP(B25,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E26" t="e">
-        <f>VLOOKUP(B26,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G26" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E27" t="e">
-        <f>VLOOKUP(B27,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E28" t="e">
-        <f>VLOOKUP(B28,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E29" t="e">
-        <f>VLOOKUP(B29,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G29" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E30" t="e">
-        <f>VLOOKUP(B30,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E31" t="e">
-        <f>VLOOKUP(B31,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G31" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E32" t="e">
-        <f>VLOOKUP(B32,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G32" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E33" t="e">
-        <f>VLOOKUP(B33,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G33" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E34" t="e">
-        <f>VLOOKUP(B34,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G34" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E35" t="e">
-        <f>VLOOKUP(B35,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G35" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E36" t="e">
-        <f>VLOOKUP(B36,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G36" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E37" t="e">
-        <f>VLOOKUP(B37,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E38" t="e">
-        <f>VLOOKUP(B38,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G38" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E39" t="e">
-        <f>VLOOKUP(B39,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G39" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E40" t="e">
-        <f>VLOOKUP(B40,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G40" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E41" t="e">
-        <f>VLOOKUP(B41,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G41" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E42" t="e">
-        <f>VLOOKUP(B42,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G42" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E43" t="e">
-        <f>VLOOKUP(B43,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G43" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E44" t="e">
-        <f>VLOOKUP(B44,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E45" t="e">
-        <f>VLOOKUP(B45,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G45" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E46" t="e">
-        <f>VLOOKUP(B46,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G46" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E47" t="e">
-        <f>VLOOKUP(B47,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G47" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E48" t="e">
-        <f>VLOOKUP(B48,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G48" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E49" t="e">
-        <f>VLOOKUP(B49,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
-      </c>
       <c r="G49" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E50" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-ALLOW", "type": "packedDecimal", "size": 5, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="str">
         <f>VLOOKUP(B50,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>string</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E51" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-ACODE", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="str">
         <f>VLOOKUP(B51,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>string</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E52" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-TCODE", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52">
+        <v>7</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" t="str">
         <f>VLOOKUP(B52,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E53" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-LIMIT", "type": "packedDecimal", "size": 7, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" t="str">
         <f>VLOOKUP(B53,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E54" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-ALLOW2", "type": "packedDecimal", "size": 5, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="str">
         <f>VLOOKUP(B54,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>string</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E55" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-ACODE2", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="str">
         <f>VLOOKUP(B55,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>string</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E56" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-TCODE2", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>132</v>
+      </c>
+      <c r="B56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56">
+        <v>7</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" t="str">
         <f>VLOOKUP(B56,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E57" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-LIMIT2", "type": "packedDecimal", "size": 7, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="E57" t="str">
         <f>VLOOKUP(B57,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>uinteger</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E58" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-DATE2", "type": "uinteger", "size": 2 },</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>134</v>
+      </c>
+      <c r="B58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58" t="str">
         <f>VLOOKUP(B58,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E59" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-ALLOW3", "type": "packedDecimal", "size": 5, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>135</v>
+      </c>
+      <c r="B59" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="str">
         <f>VLOOKUP(B59,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>string</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E60" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-ACODE3", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="str">
         <f>VLOOKUP(B60,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>string</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E61" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-TCODE3", "type": "string", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61">
+        <v>7</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61" t="str">
         <f>VLOOKUP(B61,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E62" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-LIMIT3", "type": "packedDecimal", "size": 7, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="E62" t="str">
         <f>VLOOKUP(B62,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>uinteger</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E63" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-DATE3", "type": "uinteger", "size": 2 },</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="str">
         <f>VLOOKUP(B63,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>uinteger</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E64" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-FORM-LCK", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64" t="str">
         <f>VLOOKUP(B64,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E65" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-PGT", "type": "packedDecimal", "size": 3, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>141</v>
+      </c>
+      <c r="B65" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="str">
         <f>VLOOKUP(B65,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>uinteger</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E66" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-TSWA", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>142</v>
+      </c>
+      <c r="B66" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66" t="str">
         <f>VLOOKUP(B66,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E67" t="e">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">				{ "name": "WM-EGT", "type": "packedDecimal", "size": 3, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>143</v>
+      </c>
+      <c r="B67" t="s">
+        <v>38</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="str">
         <f>VLOOKUP(B67,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>uinteger</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E68" t="e">
+        <f t="shared" ref="G67:G130" si="1">IF(LEN(A67)&gt;0,"				{ ""name"": """&amp;A67&amp;""", ""type"": """&amp;E67&amp;""", ""size"": "&amp;C67&amp;IF(LEN(D67)&gt;0,", ""scale"": "&amp;D67,"")&amp;" },","")</f>
+        <v xml:space="preserve">				{ "name": "WM-ESWA", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>144</v>
+      </c>
+      <c r="B68" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68">
+        <v>5</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68" t="str">
         <f>VLOOKUP(B68,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E69" t="e">
+        <v xml:space="preserve">				{ "name": "WM-ACRE", "type": "packedDecimal", "size": 5, "scale": 2 },</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69" t="str">
         <f>VLOOKUP(B69,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E70" t="e">
+        <v xml:space="preserve">				{ "name": "WM-POTE", "type": "packedDecimal", "size": 5, "scale": 1 },</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70" t="str">
         <f>VLOOKUP(B70,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E71" t="e">
+        <v xml:space="preserve">				{ "name": "WM-ACFT", "type": "packedDecimal", "size": 5, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71" t="str">
         <f>VLOOKUP(B71,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E72" t="e">
+        <v xml:space="preserve">				{ "name": "WM-GOR", "type": "packedDecimal", "size": 5, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="E72" t="str">
         <f>VLOOKUP(B72,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>uinteger</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E73" t="e">
+        <v xml:space="preserve">				{ "name": "WM-OTRAN-CD", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>149</v>
+      </c>
+      <c r="B73" t="s">
+        <v>30</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73" t="str">
         <f>VLOOKUP(B73,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E74" t="e">
+        <v xml:space="preserve">				{ "name": "WM-POT", "type": "packedDecimal", "size": 3, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>150</v>
+      </c>
+      <c r="B74" t="s">
+        <v>30</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74" t="str">
         <f>VLOOKUP(B74,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>packedDecimal</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E75" t="e">
+        <v xml:space="preserve">				{ "name": "WM-EOT", "type": "packedDecimal", "size": 3, "scale": 0 },</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="E75" t="str">
         <f>VLOOKUP(B75,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>uinteger</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E76" t="e">
+        <v xml:space="preserve">				{ "name": "WM-JOHN", "type": "uinteger", "size": 1 },</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76">
+        <v>6</v>
+      </c>
+      <c r="E76" t="str">
         <f>VLOOKUP(B76,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>uinteger</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E77" t="e">
+        <v xml:space="preserve">				{ "name": "WM-OOIP", "type": "uinteger", "size": 6 },</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B77" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="E77" t="str">
         <f>VLOOKUP(B77,datatypes!B:D,3,0)</f>
-        <v>#N/A</v>
+        <v>uinteger</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="78" spans="5:7" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">				{ "name": "----14-FILLER3", "type": "uinteger", "size": 3 },</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E78" t="e">
         <f>VLOOKUP(B78,datatypes!B:D,3,0)</f>
         <v>#N/A</v>
@@ -2014,7 +2874,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E79" t="e">
         <f>VLOOKUP(B79,datatypes!B:D,3,0)</f>
         <v>#N/A</v>
@@ -2024,7 +2884,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E80" t="e">
         <f>VLOOKUP(B80,datatypes!B:D,3,0)</f>
         <v>#N/A</v>
@@ -2090,7 +2950,7 @@
         <v>#N/A</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" ref="G86:G149" si="2">IF(LEN(A86)&gt;0,"				{ ""name"": """&amp;A86&amp;""", ""type"": """&amp;B86&amp;""", ""size"": "&amp;C86&amp;IF(LEN(D86)&gt;0,", ""scale"": "&amp;D86,"")&amp;" },","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2100,7 +2960,7 @@
         <v>#N/A</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2110,7 +2970,7 @@
         <v>#N/A</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2120,7 +2980,7 @@
         <v>#N/A</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2130,7 +2990,7 @@
         <v>#N/A</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2140,7 +3000,7 @@
         <v>#N/A</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2150,7 +3010,7 @@
         <v>#N/A</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2160,7 +3020,7 @@
         <v>#N/A</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2170,7 +3030,7 @@
         <v>#N/A</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2180,7 +3040,7 @@
         <v>#N/A</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2190,7 +3050,7 @@
         <v>#N/A</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2200,7 +3060,7 @@
         <v>#N/A</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2210,7 +3070,7 @@
         <v>#N/A</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2220,7 +3080,7 @@
         <v>#N/A</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2230,7 +3090,7 @@
         <v>#N/A</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2240,7 +3100,7 @@
         <v>#N/A</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2250,7 +3110,7 @@
         <v>#N/A</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2260,7 +3120,7 @@
         <v>#N/A</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2270,7 +3130,7 @@
         <v>#N/A</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2280,7 +3140,7 @@
         <v>#N/A</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2290,7 +3150,7 @@
         <v>#N/A</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2300,7 +3160,7 @@
         <v>#N/A</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2310,7 +3170,7 @@
         <v>#N/A</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2320,7 +3180,7 @@
         <v>#N/A</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2330,7 +3190,7 @@
         <v>#N/A</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2340,7 +3200,7 @@
         <v>#N/A</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2350,7 +3210,7 @@
         <v>#N/A</v>
       </c>
       <c r="G112" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2360,7 +3220,7 @@
         <v>#N/A</v>
       </c>
       <c r="G113" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2370,7 +3230,7 @@
         <v>#N/A</v>
       </c>
       <c r="G114" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2380,7 +3240,7 @@
         <v>#N/A</v>
       </c>
       <c r="G115" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2390,7 +3250,7 @@
         <v>#N/A</v>
       </c>
       <c r="G116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2400,7 +3260,7 @@
         <v>#N/A</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2410,7 +3270,7 @@
         <v>#N/A</v>
       </c>
       <c r="G118" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2420,7 +3280,7 @@
         <v>#N/A</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2430,7 +3290,7 @@
         <v>#N/A</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2440,7 +3300,7 @@
         <v>#N/A</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2450,61 +3310,61 @@
         <v>#N/A</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G123" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G124" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G126" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G127" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="128" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G128" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="129" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G129" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="130" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G130" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="131" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G131" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G131:G160" si="2">IF(LEN(A131)&gt;0,"				{ ""name"": """&amp;A131&amp;""", ""type"": """&amp;E131&amp;""", ""size"": "&amp;C131&amp;IF(LEN(D131)&gt;0,", ""scale"": "&amp;D131,"")&amp;" },","")</f>
         <v/>
       </c>
     </row>
@@ -2618,49 +3478,67 @@
     </row>
     <row r="150" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G150" t="str">
-        <f t="shared" ref="G150:G157" si="3">IF(LEN(A150)&gt;0,"				{ ""name"": """&amp;A150&amp;""", ""type"": """&amp;B150&amp;""", ""size"": "&amp;C150&amp;IF(LEN(D150)&gt;0,", ""scale"": "&amp;D150,"")&amp;" },","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="151" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G151" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="152" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G152" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="153" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G153" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="154" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G154" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="155" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G155" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="156" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G156" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="157" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G157" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="158" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G158" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="159" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G159" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G160" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -2673,9 +3551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4383763-5F97-4B63-8360-0A74869FDE3D}">
   <dimension ref="B1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>